<commit_message>
Altered code and calculated precision plus recall
</commit_message>
<xml_diff>
--- a/KTAI3.xlsx
+++ b/KTAI3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorrit/Library/Mobile Documents/com~apple~CloudDocs/Studie OU/Master/IM0712 Key Topics in Artificial Intelligence/Assignment 3/KTA3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FC013D-BBC7-C144-BF45-910AEFF5A078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE4EC88-1750-E945-A5E8-1E6CB8213678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15200" yWindow="920" windowWidth="14900" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="40">
   <si>
     <t>Cluster 0</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Cluster 0 + 8</t>
+  </si>
+  <si>
+    <t>F1 Score</t>
+  </si>
+  <si>
+    <t>F1-Score</t>
   </si>
 </sst>
 </file>
@@ -467,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -483,7 +489,7 @@
     <col min="25" max="25" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -521,7 +527,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -567,8 +573,11 @@
       <c r="R2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -616,8 +625,12 @@
         <f>B2/SUM(B2:B7)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S3">
+        <f>(2*Q3*R3)/(Q3+R3)</f>
+        <v>0.84444444444444433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -665,8 +678,12 @@
         <f>D3/SUM(D2:D7)</f>
         <v>0.85057471264367812</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S4">
+        <f t="shared" ref="S4:S7" si="0">(2*Q4*R4)/(Q4+R4)</f>
+        <v>0.88095238095238093</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -714,8 +731,12 @@
         <f>G4/SUM(G2:G7)</f>
         <v>0.99236641221374045</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>0.89655172413793116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -769,8 +790,12 @@
         <f>H5/SUM(H2:H7)</f>
         <v>0.93478260869565222</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>0.92972972972972967</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -818,8 +843,12 @@
         <f>J6/SUM(J2:J7)</f>
         <v>0.98333333333333328</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>0.6113989637305699</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -828,47 +857,47 @@
         <v>57</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:M8" si="0">SUM(C2:C7)</f>
+        <f t="shared" ref="C8:M8" si="1">SUM(C2:C7)</f>
         <v>29</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>174</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>131</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="L8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="M8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="N8">
@@ -886,8 +915,12 @@
         <f>AVERAGE(R3:R7)</f>
         <v>0.95221141337728077</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S8">
+        <f>(2*Q8*R8)/(Q8+R8)</f>
+        <v>0.84905218446722697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -936,6 +969,9 @@
       <c r="R11" t="s">
         <v>18</v>
       </c>
+      <c r="S11" t="s">
+        <v>38</v>
+      </c>
       <c r="T11" t="s">
         <v>31</v>
       </c>
@@ -960,8 +996,11 @@
       <c r="AB11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -988,6 +1027,10 @@
         <f>B18/SUM(B12:B24)</f>
         <v>1</v>
       </c>
+      <c r="S12">
+        <f t="shared" ref="S9:S25" si="2">(2*Q12*R12)/(Q12+R12)</f>
+        <v>0.82926829268292679</v>
+      </c>
       <c r="T12" t="s">
         <v>37</v>
       </c>
@@ -1002,6 +1045,10 @@
         <f>(J12+J20)/J25</f>
         <v>0.85</v>
       </c>
+      <c r="X12">
+        <f t="shared" ref="X12:X24" si="3">(2*V12*W12)/(V12+W12)</f>
+        <v>0.86440677966101698</v>
+      </c>
       <c r="Y12" t="s">
         <v>37</v>
       </c>
@@ -1016,8 +1063,12 @@
         <f>(J12+J20)/J25</f>
         <v>0.85</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC12">
+        <f t="shared" ref="AC12:AC24" si="4">(2*AA12*AB12)/(AA12+AB12)</f>
+        <v>0.86440677966101698</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1038,6 +1089,10 @@
         <f xml:space="preserve"> D13/SUM(D12:D24)</f>
         <v>0.56896551724137934</v>
       </c>
+      <c r="S13">
+        <f t="shared" si="2"/>
+        <v>0.72527472527472525</v>
+      </c>
       <c r="T13" t="s">
         <v>34</v>
       </c>
@@ -1052,6 +1107,10 @@
         <f>(D13+D15+D19)/D25</f>
         <v>0.78735632183908044</v>
       </c>
+      <c r="X13">
+        <f t="shared" si="3"/>
+        <v>0.79420289855072468</v>
+      </c>
       <c r="Y13" t="s">
         <v>35</v>
       </c>
@@ -1066,8 +1125,12 @@
         <f>(D13+D15)/D25</f>
         <v>0.73563218390804597</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC13">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1091,6 +1154,10 @@
         <f xml:space="preserve"> G14/SUM(G12:G24)</f>
         <v>0.99236641221374045</v>
       </c>
+      <c r="S14">
+        <f t="shared" si="2"/>
+        <v>0.91228070175438591</v>
+      </c>
       <c r="T14" t="s">
         <v>2</v>
       </c>
@@ -1105,6 +1172,10 @@
         <f xml:space="preserve"> G14/SUM(G12:G24)</f>
         <v>0.99236641221374045</v>
       </c>
+      <c r="X14">
+        <f t="shared" si="3"/>
+        <v>0.91228070175438591</v>
+      </c>
       <c r="Y14" t="s">
         <v>2</v>
       </c>
@@ -1119,8 +1190,12 @@
         <f xml:space="preserve"> G14/SUM(G12:G24)</f>
         <v>0.99236641221374045</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC14">
+        <f t="shared" si="4"/>
+        <v>0.91228070175438591</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1147,6 +1222,10 @@
         <f xml:space="preserve"> D15/SUM(D12:D24)</f>
         <v>0.16666666666666666</v>
       </c>
+      <c r="S15">
+        <f t="shared" si="2"/>
+        <v>0.26244343891402716</v>
+      </c>
       <c r="T15" t="s">
         <v>4</v>
       </c>
@@ -1161,6 +1240,10 @@
         <f>C16/C25</f>
         <v>0.89655172413793105</v>
       </c>
+      <c r="X15">
+        <f t="shared" si="3"/>
+        <v>0.94545454545454544</v>
+      </c>
       <c r="Y15" t="s">
         <v>4</v>
       </c>
@@ -1175,8 +1258,12 @@
         <f>C16/C25</f>
         <v>0.89655172413793105</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC15">
+        <f t="shared" si="4"/>
+        <v>0.94545454545454544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1197,6 +1284,10 @@
         <f xml:space="preserve"> C16/SUM(C12:C24)</f>
         <v>0.89655172413793105</v>
       </c>
+      <c r="S16">
+        <f t="shared" si="2"/>
+        <v>0.94545454545454544</v>
+      </c>
       <c r="T16" t="s">
         <v>22</v>
       </c>
@@ -1211,6 +1302,10 @@
         <f>H17/H25</f>
         <v>0.86956521739130432</v>
       </c>
+      <c r="X16">
+        <f t="shared" si="3"/>
+        <v>0.93023255813953487</v>
+      </c>
       <c r="Y16" t="s">
         <v>36</v>
       </c>
@@ -1225,8 +1320,12 @@
         <f>(H17+H19)/H25</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC16">
+        <f t="shared" si="4"/>
+        <v>0.93401015228426398</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1247,6 +1346,10 @@
         <f xml:space="preserve"> H17/SUM(H12:H24)</f>
         <v>0.86956521739130432</v>
       </c>
+      <c r="S17">
+        <f t="shared" si="2"/>
+        <v>0.93023255813953487</v>
+      </c>
       <c r="T17" t="s">
         <v>23</v>
       </c>
@@ -1261,6 +1364,10 @@
         <f>B18/B25</f>
         <v>1</v>
       </c>
+      <c r="X17">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="Y17" t="s">
         <v>23</v>
       </c>
@@ -1275,8 +1382,12 @@
         <f>B18/B25</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1295,6 +1406,10 @@
       </c>
       <c r="R18">
         <f xml:space="preserve"> B18/SUM(B12:B24)</f>
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="T18" t="s">
@@ -1311,6 +1426,10 @@
         <f>E21/E25</f>
         <v>1</v>
       </c>
+      <c r="X18">
+        <f t="shared" si="3"/>
+        <v>0.49180327868852458</v>
+      </c>
       <c r="Y18" t="s">
         <v>26</v>
       </c>
@@ -1325,8 +1444,12 @@
         <f>E21/E25</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC18">
+        <f t="shared" si="4"/>
+        <v>0.49180327868852458</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1353,6 +1476,10 @@
         <f>D19/D25</f>
         <v>5.1724137931034482E-2</v>
       </c>
+      <c r="S19">
+        <f t="shared" si="2"/>
+        <v>9.0452261306532666E-2</v>
+      </c>
       <c r="T19" t="s">
         <v>27</v>
       </c>
@@ -1367,6 +1494,10 @@
         <f>K22/K25</f>
         <v>1</v>
       </c>
+      <c r="X19">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="Y19" t="s">
         <v>27</v>
       </c>
@@ -1381,8 +1512,12 @@
         <f>K22/K25</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1403,6 +1538,10 @@
         <f>H19/H25</f>
         <v>0.13043478260869565</v>
       </c>
+      <c r="S20">
+        <f t="shared" si="2"/>
+        <v>0.20512820512820509</v>
+      </c>
       <c r="T20" t="s">
         <v>28</v>
       </c>
@@ -1417,6 +1556,10 @@
         <f>I23/I25</f>
         <v>1</v>
       </c>
+      <c r="X20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="Y20" t="s">
         <v>28</v>
       </c>
@@ -1431,8 +1574,12 @@
         <f>I23/I25</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1456,6 +1603,10 @@
         <f xml:space="preserve"> J20/SUM(J12:J24)</f>
         <v>0.56666666666666665</v>
       </c>
+      <c r="S21">
+        <f t="shared" si="2"/>
+        <v>0.72340425531914887</v>
+      </c>
       <c r="T21" t="s">
         <v>21</v>
       </c>
@@ -1467,6 +1618,10 @@
         <f>AVERAGE(W12:W20)</f>
         <v>0.93287107506467293</v>
       </c>
+      <c r="X21">
+        <f t="shared" si="3"/>
+        <v>0.90157067979101002</v>
+      </c>
       <c r="Y21" t="s">
         <v>21</v>
       </c>
@@ -1478,8 +1633,12 @@
         <f>AVERAGE(AB12:AB20)</f>
         <v>0.94161670225107974</v>
       </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC21">
+        <f t="shared" si="4"/>
+        <v>0.90273637784965466</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1500,8 +1659,12 @@
         <f xml:space="preserve"> E21/SUM(E12:E24)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S22">
+        <f t="shared" si="2"/>
+        <v>0.49180327868852458</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1522,8 +1685,12 @@
         <f xml:space="preserve"> K22/SUM(K12:K24)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1559,8 +1726,12 @@
         <f xml:space="preserve"> I23/SUM(I12:I24)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="S24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1569,47 +1740,47 @@
         <v>57</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:M25" si="1">SUM(C12:C24)</f>
+        <f t="shared" ref="C25:M25" si="5">SUM(C12:C24)</f>
         <v>29</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>174</v>
       </c>
       <c r="E25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="G25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>131</v>
       </c>
       <c r="H25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>92</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="J25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="K25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="L25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="M25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="N25">
@@ -1626,6 +1797,10 @@
       <c r="R25">
         <f>AVERAGE(R12:R24)</f>
         <v>0.71099547114287831</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="2"/>
+        <v>0.75067533127525232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>